<commit_message>
misc updates: - update KiCad to v6 - add SMD footprint for JTAG connector
</commit_message>
<xml_diff>
--- a/doc/BOM_n64rgbv2.1.xlsx
+++ b/doc/BOM_n64rgbv2.1.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25028"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Users\Peter\Documents\Workspaces\GitHub\n64rgb\generalRGBmod\Main-PCB\v2.1\bom\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\Peter\Documents\Workspaces\GitHub\n64rgb_project\n64rgb_pcb\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35C807CC-3CDF-4CF2-A619-85803211075C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8320F2CE-7A88-438E-BAC3-CE34FA85E471}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3420" yWindow="3420" windowWidth="28800" windowHeight="15435" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6315" yWindow="3915" windowWidth="25005" windowHeight="13980" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="MaxV Setup" sheetId="1" r:id="rId1"/>
     <sheet name="MaxII Setup" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="181029" refMode="R1C1" concurrentCalc="0"/>
+  <calcPr calcId="191029" refMode="R1C1" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="330"/>
@@ -24,7 +24,11 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
       </xcalcf:calcFeatures>
     </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
@@ -35,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="265" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="273" uniqueCount="111">
   <si>
     <t>Designator</t>
   </si>
@@ -384,6 +388,16 @@
   </si>
   <si>
     <t>C51,C52</t>
+  </si>
+  <si>
+    <t xml:space="preserve">	
+3020-10-0300-00</t>
+  </si>
+  <si>
+    <t>SMD part</t>
+  </si>
+  <si>
+    <t>THT part alternative</t>
   </si>
 </sst>
 </file>
@@ -895,7 +909,7 @@
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="42"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
@@ -909,6 +923,7 @@
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="45">
     <cellStyle name="20 % - Akzent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1233,7 +1248,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J56"/>
+  <dimension ref="A1:J57"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:B1"/>
@@ -1499,7 +1514,7 @@
         <v>5</v>
       </c>
       <c r="D18">
-        <f>$C$1*C18</f>
+        <f t="shared" ref="D18:D27" si="0">$C$1*C18</f>
         <v>15</v>
       </c>
       <c r="E18" t="s">
@@ -1522,7 +1537,7 @@
         <v>15</v>
       </c>
       <c r="D19">
-        <f>$C$1*C19</f>
+        <f t="shared" si="0"/>
         <v>45</v>
       </c>
       <c r="E19" t="s">
@@ -1545,7 +1560,7 @@
         <v>4</v>
       </c>
       <c r="D20">
-        <f>$C$1*C20</f>
+        <f t="shared" si="0"/>
         <v>12</v>
       </c>
       <c r="E20" t="s">
@@ -1568,7 +1583,7 @@
         <v>1</v>
       </c>
       <c r="D21">
-        <f>$C$1*C21</f>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="E21" t="s">
@@ -1591,7 +1606,7 @@
         <v>1</v>
       </c>
       <c r="D22">
-        <f>$C$1*C22</f>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="E22" t="s">
@@ -1614,7 +1629,7 @@
         <v>4</v>
       </c>
       <c r="D23">
-        <f>$C$1*C23</f>
+        <f t="shared" si="0"/>
         <v>12</v>
       </c>
       <c r="E23" t="s">
@@ -1640,7 +1655,7 @@
         <v>1</v>
       </c>
       <c r="D24">
-        <f>$C$1*C24</f>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="E24" t="s">
@@ -1666,7 +1681,7 @@
         <v>3</v>
       </c>
       <c r="D25">
-        <f>$C$1*C25</f>
+        <f t="shared" si="0"/>
         <v>9</v>
       </c>
       <c r="E25" t="s">
@@ -1692,7 +1707,7 @@
         <v>1</v>
       </c>
       <c r="D26">
-        <f>$C$1*C26</f>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="E26" t="s">
@@ -1718,7 +1733,7 @@
         <v>1</v>
       </c>
       <c r="D27">
-        <f>$C$1*C27</f>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="E27" t="s">
@@ -1929,11 +1944,18 @@
       <c r="A37" t="s">
         <v>65</v>
       </c>
-      <c r="B37" t="s">
-        <v>63</v>
+      <c r="B37" s="7" t="s">
+        <v>108</v>
+      </c>
+      <c r="C37">
+        <v>1</v>
       </c>
       <c r="D37">
-        <v>1</v>
+        <f>$C$1*C37</f>
+        <v>3</v>
+      </c>
+      <c r="E37" t="s">
+        <v>109</v>
       </c>
       <c r="H37" t="s">
         <v>64</v>
@@ -1942,48 +1964,57 @@
       <c r="J37" s="1"/>
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B38" t="s">
+        <v>63</v>
+      </c>
+      <c r="E38" t="s">
+        <v>110</v>
+      </c>
+      <c r="H38" t="s">
+        <v>64</v>
+      </c>
       <c r="I38" s="1"/>
       <c r="J38" s="1"/>
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A39" s="3" t="s">
-        <v>77</v>
-      </c>
       <c r="I39" s="1"/>
       <c r="J39" s="1"/>
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
-        <v>76</v>
-      </c>
-      <c r="B40" s="3" t="s">
-        <v>79</v>
-      </c>
-      <c r="C40" s="3"/>
+      <c r="A40" s="3" t="s">
+        <v>77</v>
+      </c>
       <c r="I40" s="1"/>
       <c r="J40" s="1"/>
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B41" s="3"/>
+      <c r="A41" t="s">
+        <v>76</v>
+      </c>
+      <c r="B41" s="3" t="s">
+        <v>79</v>
+      </c>
       <c r="C41" s="3"/>
       <c r="I41" s="1"/>
       <c r="J41" s="1"/>
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A42" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="B42" s="5"/>
-      <c r="C42" s="5"/>
-      <c r="D42" s="5"/>
-      <c r="E42" s="5"/>
-      <c r="F42" s="5"/>
-      <c r="G42" s="5"/>
-      <c r="H42" s="5"/>
+      <c r="B42" s="3"/>
+      <c r="C42" s="3"/>
       <c r="I42" s="1"/>
       <c r="J42" s="1"/>
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A43" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B43" s="5"/>
+      <c r="C43" s="5"/>
+      <c r="D43" s="5"/>
+      <c r="E43" s="5"/>
+      <c r="F43" s="5"/>
+      <c r="G43" s="5"/>
+      <c r="H43" s="5"/>
       <c r="I43" s="1"/>
       <c r="J43" s="1"/>
     </row>
@@ -1996,25 +2027,24 @@
       <c r="J45" s="1"/>
     </row>
     <row r="46" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="F46" s="2"/>
       <c r="I46" s="1"/>
       <c r="J46" s="1"/>
     </row>
     <row r="47" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="F47" s="2"/>
       <c r="I47" s="1"/>
       <c r="J47" s="1"/>
     </row>
     <row r="48" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="F48" s="2"/>
       <c r="I48" s="1"/>
       <c r="J48" s="1"/>
     </row>
     <row r="49" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="F49" s="2"/>
       <c r="I49" s="1"/>
       <c r="J49" s="1"/>
     </row>
     <row r="50" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="F50" s="2"/>
       <c r="I50" s="1"/>
       <c r="J50" s="1"/>
     </row>
@@ -2028,17 +2058,22 @@
       <c r="I52" s="1"/>
       <c r="J52" s="1"/>
     </row>
-    <row r="55" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B55" s="1"/>
-      <c r="C55" s="1"/>
+    <row r="53" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="F53" s="2"/>
+      <c r="I53" s="1"/>
+      <c r="J53" s="1"/>
     </row>
     <row r="56" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B56" s="1"/>
       <c r="C56" s="1"/>
     </row>
+    <row r="57" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B57" s="1"/>
+      <c r="C57" s="1"/>
+    </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="A42:H42"/>
+    <mergeCell ref="A43:H43"/>
     <mergeCell ref="A1:B1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
@@ -2048,7 +2083,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:J52"/>
+  <dimension ref="A1:J53"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection sqref="A1:B1"/>
@@ -2290,7 +2325,7 @@
         <v>5</v>
       </c>
       <c r="D17">
-        <f>$C$1*C17</f>
+        <f t="shared" ref="D17:D26" si="0">$C$1*C17</f>
         <v>15</v>
       </c>
       <c r="E17" t="s">
@@ -2313,7 +2348,7 @@
         <v>15</v>
       </c>
       <c r="D18">
-        <f>$C$1*C18</f>
+        <f t="shared" si="0"/>
         <v>45</v>
       </c>
       <c r="E18" t="s">
@@ -2336,7 +2371,7 @@
         <v>4</v>
       </c>
       <c r="D19">
-        <f>$C$1*C19</f>
+        <f t="shared" si="0"/>
         <v>12</v>
       </c>
       <c r="E19" t="s">
@@ -2359,7 +2394,7 @@
         <v>1</v>
       </c>
       <c r="D20">
-        <f>$C$1*C20</f>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="E20" t="s">
@@ -2382,7 +2417,7 @@
         <v>1</v>
       </c>
       <c r="D21">
-        <f>$C$1*C21</f>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="E21" t="s">
@@ -2405,7 +2440,7 @@
         <v>2</v>
       </c>
       <c r="D22">
-        <f>$C$1*C22</f>
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
       <c r="E22" t="s">
@@ -2431,7 +2466,7 @@
         <v>1</v>
       </c>
       <c r="D23">
-        <f>$C$1*C23</f>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="E23" t="s">
@@ -2457,7 +2492,7 @@
         <v>3</v>
       </c>
       <c r="D24">
-        <f>$C$1*C24</f>
+        <f t="shared" si="0"/>
         <v>9</v>
       </c>
       <c r="E24" t="s">
@@ -2483,7 +2518,7 @@
         <v>1</v>
       </c>
       <c r="D25">
-        <f>$C$1*C25</f>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="E25" t="s">
@@ -2509,7 +2544,7 @@
         <v>1</v>
       </c>
       <c r="D26">
-        <f>$C$1*C26</f>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="E26" t="s">
@@ -2720,11 +2755,18 @@
       <c r="A36" t="s">
         <v>65</v>
       </c>
-      <c r="B36" t="s">
-        <v>63</v>
+      <c r="B36" s="7" t="s">
+        <v>108</v>
+      </c>
+      <c r="C36">
+        <v>1</v>
       </c>
       <c r="D36">
-        <v>1</v>
+        <f>$C$1*C36</f>
+        <v>3</v>
+      </c>
+      <c r="E36" t="s">
+        <v>109</v>
       </c>
       <c r="H36" t="s">
         <v>64</v>
@@ -2733,63 +2775,71 @@
       <c r="J36" s="1"/>
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B37" t="s">
+        <v>63</v>
+      </c>
+      <c r="E37" t="s">
+        <v>110</v>
+      </c>
+      <c r="H37" t="s">
+        <v>64</v>
+      </c>
       <c r="I37" s="1"/>
       <c r="J37" s="1"/>
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A38" s="3" t="s">
+      <c r="I38" s="1"/>
+      <c r="J38" s="1"/>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A39" s="3" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
         <v>78</v>
       </c>
-      <c r="B39" s="3"/>
-      <c r="C39" s="3"/>
-      <c r="I39" s="1"/>
-      <c r="J39" s="1"/>
-    </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B40" s="3"/>
       <c r="C40" s="3"/>
       <c r="I40" s="1"/>
       <c r="J40" s="1"/>
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A41" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="B41" s="5"/>
-      <c r="C41" s="5"/>
-      <c r="D41" s="5"/>
-      <c r="E41" s="5"/>
-      <c r="F41" s="5"/>
-      <c r="G41" s="5"/>
-      <c r="H41" s="5"/>
+      <c r="B41" s="3"/>
+      <c r="C41" s="3"/>
       <c r="I41" s="1"/>
       <c r="J41" s="1"/>
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="F42" s="2"/>
+      <c r="A42" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B42" s="5"/>
+      <c r="C42" s="5"/>
+      <c r="D42" s="5"/>
+      <c r="E42" s="5"/>
+      <c r="F42" s="5"/>
+      <c r="G42" s="5"/>
+      <c r="H42" s="5"/>
       <c r="I42" s="1"/>
       <c r="J42" s="1"/>
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="F43" s="2"/>
       <c r="I43" s="1"/>
       <c r="J43" s="1"/>
     </row>
     <row r="44" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="F44" s="2"/>
       <c r="I44" s="1"/>
       <c r="J44" s="1"/>
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="F45" s="2"/>
       <c r="I45" s="1"/>
       <c r="J45" s="1"/>
     </row>
     <row r="46" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="F46" s="2"/>
       <c r="I46" s="1"/>
       <c r="J46" s="1"/>
     </row>
@@ -2803,18 +2853,23 @@
       <c r="I48" s="1"/>
       <c r="J48" s="1"/>
     </row>
-    <row r="51" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B51" s="1"/>
-      <c r="C51" s="1"/>
-    </row>
-    <row r="52" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="49" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="F49" s="2"/>
+      <c r="I49" s="1"/>
+      <c r="J49" s="1"/>
+    </row>
+    <row r="52" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B52" s="1"/>
       <c r="C52" s="1"/>
+    </row>
+    <row r="53" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B53" s="1"/>
+      <c r="C53" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="A1:B1"/>
-    <mergeCell ref="A41:H41"/>
+    <mergeCell ref="A42:H42"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>

</xml_diff>